<commit_message>
adding sprites lasting canon
</commit_message>
<xml_diff>
--- a/Diseño/Cronograma.xlsx
+++ b/Diseño/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\Documentos\GENIALITYXD USB\UDEA\SEMESTRE II\Informática II\Proyecto Final\Repositorio Proyecto\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5F38D2-9D47-4EA1-9C59-B175062B4138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C845C1DF-5DC9-4199-A631-58C8B46D6303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
   </bookViews>
@@ -142,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -355,6 +361,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,8 +375,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E7B29F-2462-4AC8-8F0D-A242710021C1}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,33 +711,33 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="17" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="18"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -738,10 +746,10 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1"/>
+      <c r="C2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="15"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -771,10 +779,10 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -808,10 +816,10 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="14"/>
@@ -851,8 +859,8 @@
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -888,8 +896,8 @@
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -925,8 +933,8 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
@@ -962,8 +970,8 @@
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="14"/>
       <c r="F8" s="1" t="s">
         <v>6</v>
@@ -999,8 +1007,8 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="14"/>
       <c r="F9" s="1"/>
       <c r="G9" s="14" t="s">
@@ -1038,8 +1046,8 @@
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="14"/>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -1077,10 +1085,10 @@
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="14" t="s">
@@ -1122,8 +1130,8 @@
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1157,8 +1165,8 @@
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1192,8 +1200,8 @@
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1229,8 +1237,8 @@
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1268,8 +1276,8 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="1"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1305,8 +1313,8 @@
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="1"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1344,8 +1352,8 @@
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1391,8 +1399,8 @@
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
         <v>6</v>
@@ -1440,8 +1448,8 @@
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1479,8 +1487,8 @@
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1516,8 +1524,8 @@
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="1"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1555,8 +1563,8 @@
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="1"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
         <v>6</v>
@@ -1604,8 +1612,8 @@
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="1"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1647,8 +1655,8 @@
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1690,10 +1698,10 @@
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="1"/>
@@ -1737,8 +1745,8 @@
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
         <v>6</v>
@@ -1796,10 +1804,10 @@
       <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">

</xml_diff>

<commit_message>
Modificacion sprites + avance map 1
</commit_message>
<xml_diff>
--- a/Diseño/Cronograma.xlsx
+++ b/Diseño/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\Documentos\GENIALITYXD USB\UDEA\SEMESTRE II\Informática II\Proyecto Final\Repositorio Proyecto\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C845C1DF-5DC9-4199-A631-58C8B46D6303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD3ADA-21E3-4F03-BA8E-82C111F03114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
   </bookViews>
@@ -363,6 +363,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,8 +377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E7B29F-2462-4AC8-8F0D-A242710021C1}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,33 +711,33 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="19" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="20"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -746,12 +746,12 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
@@ -779,16 +779,16 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="C3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
@@ -816,14 +816,14 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="C4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="6" t="s">
@@ -859,14 +859,14 @@
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="1"/>
@@ -896,14 +896,14 @@
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="1"/>
@@ -933,12 +933,12 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="14" t="s">
@@ -970,10 +970,10 @@
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="1" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="14" t="s">
@@ -1007,10 +1007,10 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
@@ -1046,10 +1046,10 @@
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="1" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="14" t="s">
@@ -1085,16 +1085,16 @@
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="14" t="s">
+      <c r="C11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="14" t="s">
@@ -1130,10 +1130,10 @@
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
@@ -1165,10 +1165,10 @@
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
@@ -1200,10 +1200,10 @@
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="6" t="s">
@@ -1237,10 +1237,10 @@
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
@@ -1276,10 +1276,10 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
@@ -1313,10 +1313,10 @@
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="6" t="s">
@@ -1352,10 +1352,10 @@
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="1"/>
       <c r="H18" s="14" t="s">
         <v>6</v>
@@ -1399,10 +1399,10 @@
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="14" t="s">
@@ -1448,10 +1448,10 @@
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
@@ -1487,10 +1487,10 @@
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="6"/>
@@ -1524,10 +1524,10 @@
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="6"/>
@@ -1563,10 +1563,10 @@
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1612,10 +1612,10 @@
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
@@ -1655,10 +1655,10 @@
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="6"/>
@@ -1698,14 +1698,14 @@
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="C26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
@@ -1745,10 +1745,10 @@
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -1804,16 +1804,16 @@
       <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="C28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="3" t="s">

</xml_diff>

<commit_message>
lvl1 completed + falta mov auto plats
</commit_message>
<xml_diff>
--- a/Diseño/Cronograma.xlsx
+++ b/Diseño/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\Documentos\GENIALITYXD USB\UDEA\SEMESTRE II\Informática II\Proyecto Final\Repositorio Proyecto\Diseño\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD3ADA-21E3-4F03-BA8E-82C111F03114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8583367-6A8F-4119-982B-93B74403E643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -377,6 +377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E7B29F-2462-4AC8-8F0D-A242710021C1}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,16 +755,16 @@
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="15"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="1"/>
@@ -788,16 +792,16 @@
       <c r="E3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="15"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="1"/>
@@ -823,24 +827,24 @@
         <v>6</v>
       </c>
       <c r="E4" s="17"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="1"/>
@@ -866,18 +870,18 @@
       <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="F5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="1"/>
@@ -903,18 +907,18 @@
       <c r="E6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="F6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="15"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="1"/>
@@ -938,20 +942,20 @@
       <c r="E7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="F7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="15"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="1"/>
@@ -973,22 +977,22 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="F8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="1"/>
@@ -1010,24 +1014,24 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="15"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="1"/>
@@ -1049,24 +1053,24 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="F10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="1"/>
@@ -1094,24 +1098,24 @@
       <c r="E11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="F11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="15"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="1"/>
@@ -1133,16 +1137,16 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="1"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="15"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="5" t="s">
         <v>6</v>
@@ -1168,16 +1172,16 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="15"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="14"/>
@@ -1203,22 +1207,22 @@
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="15"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="1"/>
@@ -1240,24 +1244,24 @@
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="1"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="15"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="1"/>
@@ -1279,22 +1283,22 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="17"/>
+      <c r="O16" s="15"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="1"/>
@@ -1316,24 +1320,24 @@
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P17" s="6"/>
@@ -1355,30 +1359,30 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O18" s="1"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="15"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="1"/>
@@ -1402,32 +1406,32 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="F19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="17"/>
+      <c r="O19" s="15"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="1"/>
@@ -1451,20 +1455,20 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="1" t="s">
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P20" s="6"/>
@@ -1490,16 +1494,16 @@
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="15"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="1" t="s">
@@ -1527,16 +1531,16 @@
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="15"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="1"/>
@@ -1566,32 +1570,32 @@
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N23" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O23" s="14" t="s">
+      <c r="F23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P23" s="6"/>
@@ -1615,20 +1619,20 @@
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P24" s="6"/>
@@ -1658,18 +1662,18 @@
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O25" s="1" t="s">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P25" s="6" t="s">
@@ -1705,18 +1709,18 @@
         <v>6</v>
       </c>
       <c r="E26" s="17"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O26" s="14" t="s">
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P26" s="6" t="s">
@@ -1748,34 +1752,34 @@
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" s="14" t="s">
+      <c r="F27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P27" s="6" t="s">
@@ -1813,34 +1817,34 @@
       <c r="E28" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O28" s="3" t="s">
+      <c r="F28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="16" t="s">
         <v>6</v>
       </c>
       <c r="P28" s="8" t="s">

</xml_diff>

<commit_message>
lvl 2 completed + fin all interacts + esquema map 3
</commit_message>
<xml_diff>
--- a/Diseño/Cronograma.xlsx
+++ b/Diseño/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8583367-6A8F-4119-982B-93B74403E643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DEB664-AD76-4929-BD3D-07446AC43301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{743588E9-A301-49AA-ACA7-1819784143A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -345,26 +345,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,10 +377,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E7B29F-2462-4AC8-8F0D-A242710021C1}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,10 +707,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="19" t="s">
@@ -744,410 +742,410 @@
       <c r="W1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="6"/>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="23"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="6"/>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="23"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="6"/>
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="23"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
-      <c r="W4" s="11" t="s">
+      <c r="W4" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="6"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="23"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="11" t="s">
+      <c r="W5" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="6"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="23"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="11" t="s">
+      <c r="W6" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="6"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-      <c r="W7" s="11" t="s">
+      <c r="W7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="6"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="23"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
-      <c r="W8" s="11" t="s">
+      <c r="W8" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="6"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-      <c r="W9" s="11" t="s">
+      <c r="W9" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="6"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="11" t="s">
+      <c r="W10" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="6"/>
+      <c r="C11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="11" t="s">
+      <c r="W11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="6"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="23"/>
       <c r="Q12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1158,33 +1156,33 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="11" t="s">
+      <c r="W12" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="6"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="23"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="14"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1" t="s">
         <v>6</v>
@@ -1193,197 +1191,197 @@
         <v>6</v>
       </c>
       <c r="V13" s="1"/>
-      <c r="W13" s="11" t="s">
+      <c r="W13" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="6"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="23"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="W14" s="11" t="s">
+      <c r="W14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="6"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="13"/>
+      <c r="P15" s="23"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="11" t="s">
+      <c r="W15" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="6"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="23"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-      <c r="W16" s="11" t="s">
+      <c r="W16" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P17" s="6"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="23"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="11"/>
+      <c r="W17" s="9"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="6"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="13"/>
+      <c r="P18" s="23"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1392,47 +1390,47 @@
       <c r="V18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="W18" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="6"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="23"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1441,37 +1439,37 @@
       <c r="V19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W19" s="11" t="s">
+      <c r="W19" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="6"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="23"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -1480,31 +1478,31 @@
       <c r="V20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W20" s="11" t="s">
+      <c r="W20" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="6"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="1" t="s">
         <v>6</v>
@@ -1517,31 +1515,31 @@
       <c r="V21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W21" s="11" t="s">
+      <c r="W21" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="6"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1" t="s">
@@ -1553,89 +1551,89 @@
       <c r="U22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="W22" s="11" t="s">
+      <c r="V22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="W22" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P23" s="6"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P23" s="23"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-      <c r="W23" s="11" t="s">
+      <c r="W23" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="6"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="23"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1" t="s">
@@ -1648,40 +1646,40 @@
       <c r="V24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W24" s="11" t="s">
+      <c r="W24" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O25" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="6" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P25" s="23" t="s">
         <v>6</v>
       </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="14" t="s">
+      <c r="S25" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T25" s="1"/>
@@ -1691,166 +1689,166 @@
       <c r="V25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W25" s="11" t="s">
+      <c r="W25" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O26" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P26" s="6" t="s">
+      <c r="C26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P26" s="23" t="s">
         <v>6</v>
       </c>
       <c r="Q26" s="5"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="14" t="s">
+      <c r="S26" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T26" s="1"/>
-      <c r="U26" s="14" t="s">
+      <c r="U26" s="12" t="s">
         <v>6</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W26" s="11" t="s">
+      <c r="W26" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P27" s="6" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P27" s="23" t="s">
         <v>6</v>
       </c>
       <c r="Q27" s="5"/>
       <c r="R27" s="1"/>
-      <c r="S27" s="14" t="s">
+      <c r="S27" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T27" s="1"/>
-      <c r="U27" s="14" t="s">
+      <c r="U27" s="12" t="s">
         <v>6</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W27" s="11" t="s">
+      <c r="W27" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="M28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="N28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="O28" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q28" s="7" t="s">
+      <c r="C28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="P28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="6" t="s">
         <v>6</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -1868,7 +1866,7 @@
       <c r="V28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="W28" s="12" t="s">
+      <c r="W28" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>